<commit_message>
preparing everything for apprisal and extraction
</commit_message>
<xml_diff>
--- a/5_Snowballing/Merged_Studies_3.xlsx
+++ b/5_Snowballing/Merged_Studies_3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antoniotrovato/Documents/GitHub/RegressionTestingOptimizationSLR/5_Snowballing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B6C91F-88ED-7740-B534-FF6C9A317434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58CC76A7-E7CA-B946-A7A1-7C045F22883B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="520" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1775" uniqueCount="1318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1765" uniqueCount="1310">
   <si>
     <t>ID</t>
   </si>
@@ -3115,18 +3115,6 @@
   </si>
   <si>
     <t>Regression testing tasks of test case prioritization, test suite reduction/minimization, and regression test selection are typically centered around criteria that are based on code coverage, test execution costs, and code modifications. Researchers have developed and evaluated new individual criteria; others have combined existing criteria in different ways to form what we--and some others--call hybrid criteria. In this paper, we formalize the notion of combining multiple criteria into a hybrid. Our goal is to create a uniform representation of such combinations so that they can be described unambiguously and shared among researchers. We envision that such sharing will allow researchers to implement, study, extend, and evaluate the hybrids using a common set of techniques and tools. We precisely formulate three hybrid combinations, Rank, Merge, and Choice, and demonstrate their usefulness in two ways. First, we recast, in terms of our formulations, others' previously reported work on hybrid criteria. Second, we use our previous results on test case prioritization to create and evaluate new hybrid criteria. Our findings suggest that hybrid criteria of others can be described using our Merge and Rank formulations, and that the hybrid criteria we developed most often outperformed their constituent individual criteria.</t>
-  </si>
-  <si>
-    <t>N Sethi, S Rani, P Singh</t>
-  </si>
-  <si>
-    <t>International journal of computer applications, 2014</t>
-  </si>
-  <si>
-    <t>Ants optimization for minimal test case selection and prioritization as to reduce the cost of regression testing</t>
-  </si>
-  <si>
-    <t>Software testing is the major process in software development life cycle. Regression testing is very costly and inevitable activity that is to be performed in a restricted environment to ensure the validity of modified software. It is inefficient to rerun every test case from test suite when some kind of modification is done in the software. Test case selection and prioritization techniques select and organize the test cases in a test suite based on some criteria such that the faults are covered quickly with minimum execution time. This task can be done on basis of the Ant Colony Optimization technique (ACO) of Swarm Intelligence as it is not deeply studied yet. The main objective of this thesis is to solve the path problem: Means to find the shortest path and Resolve the time problem: Means to minimize the time of finding shortest path. Because of time and cost constraint, it is not possible to perform extensive regression testing. Techniques such as test case selection and prioritization are used to solve the problem of time and cost constraints. In this paper we are modifying the previous technique to get better results in case of execution time and then the Effectiveness of techniques is checked with the help of APFD metric.</t>
   </si>
   <si>
     <t>PK Mishra, B Pattanaik</t>
@@ -3575,18 +3563,6 @@
   </si>
   <si>
     <t>In recent years, researchers have intensively investigated various topics in test prioritization, which aims to re-order tests to increase the rate of fault detection during regression testing. While the main research focus in test prioritization is on proposing novel prioritization techniques and evaluating on more and larger subject systems, little effort has been put on investigating the threats to validity in existing work on test prioritization. One main threat to validity is that existing work mainly evaluates prioritization techniques based on simple artificial changes on the source code and tests. For example, the changes in the source code usually include only seeded program faults, whereas the test suite is usually not augmented at all. On the contrary, in real-world software development, software systems usually undergo various changes on the source code and test suite augmentation. Therefore, it is not clear whether the conclusions drawn by existing work in test prioritization from the artificial changes are still valid for real-world software evolution. In this paper, we present the first empirical study to investigate this important threat to validity in test prioritization. We reimplemented 24 variant techniques of both the traditional and time-aware test prioritization, and investigated the impacts of software evolution on those techniques based on the version history of 8 real-world Java programs from GitHub. The results show that for both traditional and time-aware test prioritization, test suite augmentation significantly hampers their effectiveness, whereas source code changes alone do not influence their effectiveness much.</t>
-  </si>
-  <si>
-    <t>L Mei, Y Cai, C Jia, B Jiang, WK Chan</t>
-  </si>
-  <si>
-    <t>International Journal of Web Services Research (IJWSR), 2013</t>
-  </si>
-  <si>
-    <t>Test pair selection for test case prioritization in regression testing for WS-BPEL programs</t>
-  </si>
-  <si>
-    <t>Many web services not only communicate through XML-based messages, but also may dynamically modify their behaviors by applying different interpretations on XML messages through updating the associated XML Schemas or XML-based interface specifications. Such artifacts are usually complex, allowing XML-based messages conforming to these specifications structurally complex. Testing should cost-effectively cover all scenarios. Test case prioritization is a dimension of regression testing that assures a program from unintended modifications by reordering the test cases within a test suite. However, many existing test case prioritization techniques for regression testing treat test cases of different complexity generically. In this paper, the authors exploit the insights on the structural similarity of XML-based artifacts between test cases in both static and dynamic dimensions, and propose a family of test case prioritization techniques that selects pairs of test case without replacement in turn. To the best of their knowledge, it is the first test case prioritization proposal that selects test case pairs for prioritization. The authors validate their techniques by a suite of benchmarks. The empirical results show that when incorporating all dimensions, some members of our technique family can be more effective than conventional coverage-based techniques.</t>
   </si>
   <si>
     <t>F Altiero, A Corazza, S Di Martino, A Peron, LLL Starace</t>
@@ -4412,10 +4388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AN207"/>
+  <dimension ref="A1:AN205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="A113" sqref="A113:XFD113"/>
+    <sheetView tabSelected="1" topLeftCell="A193" workbookViewId="0">
+      <selection activeCell="A168" sqref="A168:XFD168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9619,7 +9595,7 @@
         <v>1029</v>
       </c>
       <c r="F132">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="J132" t="s">
         <v>1030</v>
@@ -9639,7 +9615,7 @@
         <v>1033</v>
       </c>
       <c r="F133">
-        <v>2013</v>
+        <v>2018</v>
       </c>
       <c r="J133" t="s">
         <v>1034</v>
@@ -9659,7 +9635,7 @@
         <v>1037</v>
       </c>
       <c r="F134">
-        <v>2018</v>
+        <v>2021</v>
       </c>
       <c r="J134" t="s">
         <v>1038</v>
@@ -9679,7 +9655,7 @@
         <v>1041</v>
       </c>
       <c r="F135">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="J135" t="s">
         <v>1042</v>
@@ -9699,7 +9675,7 @@
         <v>1045</v>
       </c>
       <c r="F136">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="J136" t="s">
         <v>1046</v>
@@ -9719,7 +9695,7 @@
         <v>1049</v>
       </c>
       <c r="F137">
-        <v>2022</v>
+        <v>2019</v>
       </c>
       <c r="J137" t="s">
         <v>1050</v>
@@ -9739,7 +9715,7 @@
         <v>1053</v>
       </c>
       <c r="F138">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="J138" t="s">
         <v>1054</v>
@@ -9759,7 +9735,7 @@
         <v>1057</v>
       </c>
       <c r="F139">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="J139" t="s">
         <v>1058</v>
@@ -9776,13 +9752,13 @@
         <v>1060</v>
       </c>
       <c r="E140" t="s">
+        <v>357</v>
+      </c>
+      <c r="F140">
+        <v>2019</v>
+      </c>
+      <c r="J140" t="s">
         <v>1061</v>
-      </c>
-      <c r="F140">
-        <v>2021</v>
-      </c>
-      <c r="J140" t="s">
-        <v>1062</v>
       </c>
       <c r="AN140" t="s">
         <v>944</v>
@@ -9790,16 +9766,16 @@
     </row>
     <row r="141" spans="3:40" x14ac:dyDescent="0.2">
       <c r="C141" t="s">
+        <v>1062</v>
+      </c>
+      <c r="D141" t="s">
         <v>1063</v>
       </c>
-      <c r="D141" t="s">
+      <c r="E141" t="s">
         <v>1064</v>
       </c>
-      <c r="E141" t="s">
-        <v>357</v>
-      </c>
       <c r="F141">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="J141" t="s">
         <v>1065</v>
@@ -9819,7 +9795,7 @@
         <v>1068</v>
       </c>
       <c r="F142">
-        <v>2018</v>
+        <v>2021</v>
       </c>
       <c r="J142" t="s">
         <v>1069</v>
@@ -9839,7 +9815,7 @@
         <v>1072</v>
       </c>
       <c r="F143">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="J143" t="s">
         <v>1073</v>
@@ -9859,7 +9835,7 @@
         <v>1076</v>
       </c>
       <c r="F144">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="J144" t="s">
         <v>1077</v>
@@ -9879,7 +9855,7 @@
         <v>1080</v>
       </c>
       <c r="F145">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="J145" t="s">
         <v>1081</v>
@@ -9899,7 +9875,7 @@
         <v>1084</v>
       </c>
       <c r="F146">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="J146" t="s">
         <v>1085</v>
@@ -9939,7 +9915,7 @@
         <v>1092</v>
       </c>
       <c r="F148">
-        <v>2017</v>
+        <v>2014</v>
       </c>
       <c r="J148" t="s">
         <v>1093</v>
@@ -9979,7 +9955,7 @@
         <v>1100</v>
       </c>
       <c r="F150">
-        <v>2014</v>
+        <v>2018</v>
       </c>
       <c r="J150" t="s">
         <v>1101</v>
@@ -9999,7 +9975,7 @@
         <v>1104</v>
       </c>
       <c r="F151">
-        <v>2018</v>
+        <v>2023</v>
       </c>
       <c r="J151" t="s">
         <v>1105</v>
@@ -10019,7 +9995,7 @@
         <v>1108</v>
       </c>
       <c r="F152">
-        <v>2023</v>
+        <v>2014</v>
       </c>
       <c r="J152" t="s">
         <v>1109</v>
@@ -10039,7 +10015,7 @@
         <v>1112</v>
       </c>
       <c r="F153">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="J153" t="s">
         <v>1113</v>
@@ -10059,7 +10035,7 @@
         <v>1116</v>
       </c>
       <c r="F154">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="J154" t="s">
         <v>1117</v>
@@ -10079,7 +10055,7 @@
         <v>1120</v>
       </c>
       <c r="F155">
-        <v>2014</v>
+        <v>2021</v>
       </c>
       <c r="J155" t="s">
         <v>1121</v>
@@ -10099,7 +10075,7 @@
         <v>1124</v>
       </c>
       <c r="F156">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="J156" t="s">
         <v>1125</v>
@@ -10119,7 +10095,7 @@
         <v>1128</v>
       </c>
       <c r="F157">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="J157" t="s">
         <v>1129</v>
@@ -10139,7 +10115,7 @@
         <v>1132</v>
       </c>
       <c r="F158">
-        <v>2022</v>
+        <v>2016</v>
       </c>
       <c r="J158" t="s">
         <v>1133</v>
@@ -10159,7 +10135,7 @@
         <v>1136</v>
       </c>
       <c r="F159">
-        <v>2016</v>
+        <v>2020</v>
       </c>
       <c r="J159" t="s">
         <v>1137</v>
@@ -10173,16 +10149,16 @@
         <v>1138</v>
       </c>
       <c r="D160" t="s">
+        <v>1036</v>
+      </c>
+      <c r="E160" t="s">
         <v>1139</v>
       </c>
-      <c r="E160" t="s">
+      <c r="F160">
+        <v>2015</v>
+      </c>
+      <c r="J160" t="s">
         <v>1140</v>
-      </c>
-      <c r="F160">
-        <v>2020</v>
-      </c>
-      <c r="J160" t="s">
-        <v>1141</v>
       </c>
       <c r="AN160" t="s">
         <v>944</v>
@@ -10190,16 +10166,16 @@
     </row>
     <row r="161" spans="3:40" x14ac:dyDescent="0.2">
       <c r="C161" t="s">
+        <v>1141</v>
+      </c>
+      <c r="D161" t="s">
         <v>1142</v>
-      </c>
-      <c r="D161" t="s">
-        <v>1040</v>
       </c>
       <c r="E161" t="s">
         <v>1143</v>
       </c>
       <c r="F161">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="J161" t="s">
         <v>1144</v>
@@ -10213,16 +10189,16 @@
         <v>1145</v>
       </c>
       <c r="D162" t="s">
+        <v>1036</v>
+      </c>
+      <c r="E162" t="s">
         <v>1146</v>
       </c>
-      <c r="E162" t="s">
+      <c r="F162">
+        <v>2022</v>
+      </c>
+      <c r="J162" t="s">
         <v>1147</v>
-      </c>
-      <c r="F162">
-        <v>2016</v>
-      </c>
-      <c r="J162" t="s">
-        <v>1148</v>
       </c>
       <c r="AN162" t="s">
         <v>944</v>
@@ -10230,19 +10206,19 @@
     </row>
     <row r="163" spans="3:40" x14ac:dyDescent="0.2">
       <c r="C163" t="s">
+        <v>1148</v>
+      </c>
+      <c r="D163" t="s">
+        <v>1036</v>
+      </c>
+      <c r="E163" t="s">
         <v>1149</v>
-      </c>
-      <c r="D163" t="s">
-        <v>1040</v>
-      </c>
-      <c r="E163" t="s">
-        <v>1150</v>
       </c>
       <c r="F163">
         <v>2022</v>
       </c>
       <c r="J163" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="AN163" t="s">
         <v>944</v>
@@ -10250,16 +10226,16 @@
     </row>
     <row r="164" spans="3:40" x14ac:dyDescent="0.2">
       <c r="C164" t="s">
+        <v>1151</v>
+      </c>
+      <c r="D164" t="s">
         <v>1152</v>
-      </c>
-      <c r="D164" t="s">
-        <v>1040</v>
       </c>
       <c r="E164" t="s">
         <v>1153</v>
       </c>
       <c r="F164">
-        <v>2022</v>
+        <v>2024</v>
       </c>
       <c r="J164" t="s">
         <v>1154</v>
@@ -10279,7 +10255,7 @@
         <v>1157</v>
       </c>
       <c r="F165">
-        <v>2024</v>
+        <v>2015</v>
       </c>
       <c r="J165" t="s">
         <v>1158</v>
@@ -10299,7 +10275,7 @@
         <v>1161</v>
       </c>
       <c r="F166">
-        <v>2015</v>
+        <v>2018</v>
       </c>
       <c r="J166" t="s">
         <v>1162</v>
@@ -10313,16 +10289,16 @@
         <v>1163</v>
       </c>
       <c r="D167" t="s">
+        <v>996</v>
+      </c>
+      <c r="E167" t="s">
         <v>1164</v>
       </c>
-      <c r="E167" t="s">
+      <c r="F167">
+        <v>2016</v>
+      </c>
+      <c r="J167" t="s">
         <v>1165</v>
-      </c>
-      <c r="F167">
-        <v>2018</v>
-      </c>
-      <c r="J167" t="s">
-        <v>1166</v>
       </c>
       <c r="AN167" t="s">
         <v>944</v>
@@ -10330,16 +10306,16 @@
     </row>
     <row r="168" spans="3:40" x14ac:dyDescent="0.2">
       <c r="C168" t="s">
+        <v>1166</v>
+      </c>
+      <c r="D168" t="s">
         <v>1167</v>
-      </c>
-      <c r="D168" t="s">
-        <v>996</v>
       </c>
       <c r="E168" t="s">
         <v>1168</v>
       </c>
       <c r="F168">
-        <v>2016</v>
+        <v>2020</v>
       </c>
       <c r="J168" t="s">
         <v>1169</v>
@@ -10359,7 +10335,7 @@
         <v>1172</v>
       </c>
       <c r="F169">
-        <v>2013</v>
+        <v>2015</v>
       </c>
       <c r="J169" t="s">
         <v>1173</v>
@@ -10379,7 +10355,7 @@
         <v>1176</v>
       </c>
       <c r="F170">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="J170" t="s">
         <v>1177</v>
@@ -10393,16 +10369,16 @@
         <v>1178</v>
       </c>
       <c r="D171" t="s">
+        <v>1142</v>
+      </c>
+      <c r="E171" t="s">
         <v>1179</v>
       </c>
-      <c r="E171" t="s">
+      <c r="F171">
+        <v>2016</v>
+      </c>
+      <c r="J171" t="s">
         <v>1180</v>
-      </c>
-      <c r="F171">
-        <v>2015</v>
-      </c>
-      <c r="J171" t="s">
-        <v>1181</v>
       </c>
       <c r="AN171" t="s">
         <v>944</v>
@@ -10410,19 +10386,19 @@
     </row>
     <row r="172" spans="3:40" x14ac:dyDescent="0.2">
       <c r="C172" t="s">
+        <v>1181</v>
+      </c>
+      <c r="D172" t="s">
         <v>1182</v>
       </c>
-      <c r="D172" t="s">
+      <c r="E172" t="s">
         <v>1183</v>
       </c>
-      <c r="E172" t="s">
+      <c r="F172">
+        <v>2018</v>
+      </c>
+      <c r="J172" t="s">
         <v>1184</v>
-      </c>
-      <c r="F172">
-        <v>2019</v>
-      </c>
-      <c r="J172" t="s">
-        <v>1185</v>
       </c>
       <c r="AN172" t="s">
         <v>944</v>
@@ -10430,19 +10406,19 @@
     </row>
     <row r="173" spans="3:40" x14ac:dyDescent="0.2">
       <c r="C173" t="s">
+        <v>1185</v>
+      </c>
+      <c r="D173" t="s">
+        <v>816</v>
+      </c>
+      <c r="E173" t="s">
         <v>1186</v>
       </c>
-      <c r="D173" t="s">
-        <v>1146</v>
-      </c>
-      <c r="E173" t="s">
+      <c r="F173">
+        <v>2021</v>
+      </c>
+      <c r="J173" t="s">
         <v>1187</v>
-      </c>
-      <c r="F173">
-        <v>2016</v>
-      </c>
-      <c r="J173" t="s">
-        <v>1188</v>
       </c>
       <c r="AN173" t="s">
         <v>944</v>
@@ -10450,19 +10426,19 @@
     </row>
     <row r="174" spans="3:40" x14ac:dyDescent="0.2">
       <c r="C174" t="s">
+        <v>1188</v>
+      </c>
+      <c r="D174" t="s">
         <v>1189</v>
       </c>
-      <c r="D174" t="s">
+      <c r="E174" t="s">
         <v>1190</v>
       </c>
-      <c r="E174" t="s">
+      <c r="F174">
+        <v>2024</v>
+      </c>
+      <c r="J174" t="s">
         <v>1191</v>
-      </c>
-      <c r="F174">
-        <v>2018</v>
-      </c>
-      <c r="J174" t="s">
-        <v>1192</v>
       </c>
       <c r="AN174" t="s">
         <v>944</v>
@@ -10470,22 +10446,22 @@
     </row>
     <row r="175" spans="3:40" x14ac:dyDescent="0.2">
       <c r="C175" t="s">
+        <v>1192</v>
+      </c>
+      <c r="D175" t="s">
         <v>1193</v>
-      </c>
-      <c r="D175" t="s">
-        <v>816</v>
       </c>
       <c r="E175" t="s">
         <v>1194</v>
       </c>
       <c r="F175">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="J175" t="s">
         <v>1195</v>
       </c>
       <c r="AN175" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="176" spans="3:40" x14ac:dyDescent="0.2">
@@ -10519,13 +10495,13 @@
         <v>1202</v>
       </c>
       <c r="F177">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="J177" t="s">
         <v>1203</v>
       </c>
       <c r="AN177" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
     </row>
     <row r="178" spans="3:40" x14ac:dyDescent="0.2">
@@ -10539,7 +10515,7 @@
         <v>1206</v>
       </c>
       <c r="F178">
-        <v>2024</v>
+        <v>2019</v>
       </c>
       <c r="J178" t="s">
         <v>1207</v>
@@ -10559,7 +10535,7 @@
         <v>1210</v>
       </c>
       <c r="F179">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="J179" t="s">
         <v>1211</v>
@@ -10579,7 +10555,7 @@
         <v>1214</v>
       </c>
       <c r="F180">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="J180" t="s">
         <v>1215</v>
@@ -10599,13 +10575,13 @@
         <v>1218</v>
       </c>
       <c r="F181">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="J181" t="s">
         <v>1219</v>
       </c>
       <c r="AN181" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
     </row>
     <row r="182" spans="3:40" x14ac:dyDescent="0.2">
@@ -10619,13 +10595,13 @@
         <v>1222</v>
       </c>
       <c r="F182">
-        <v>2017</v>
+        <v>2021</v>
       </c>
       <c r="J182" t="s">
         <v>1223</v>
       </c>
       <c r="AN182" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="183" spans="3:40" x14ac:dyDescent="0.2">
@@ -10639,13 +10615,13 @@
         <v>1226</v>
       </c>
       <c r="F183">
-        <v>2021</v>
+        <v>2017</v>
       </c>
       <c r="J183" t="s">
         <v>1227</v>
       </c>
       <c r="AN183" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
     </row>
     <row r="184" spans="3:40" x14ac:dyDescent="0.2">
@@ -10659,13 +10635,13 @@
         <v>1230</v>
       </c>
       <c r="F184">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="J184" t="s">
         <v>1231</v>
       </c>
       <c r="AN184" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
     </row>
     <row r="185" spans="3:40" x14ac:dyDescent="0.2">
@@ -10679,13 +10655,13 @@
         <v>1234</v>
       </c>
       <c r="F185">
-        <v>2017</v>
+        <v>2021</v>
       </c>
       <c r="J185" t="s">
         <v>1235</v>
       </c>
       <c r="AN185" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
     </row>
     <row r="186" spans="3:40" x14ac:dyDescent="0.2">
@@ -10699,7 +10675,7 @@
         <v>1238</v>
       </c>
       <c r="F186">
-        <v>2024</v>
+        <v>2019</v>
       </c>
       <c r="J186" t="s">
         <v>1239</v>
@@ -10719,7 +10695,7 @@
         <v>1242</v>
       </c>
       <c r="F187">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="J187" t="s">
         <v>1243</v>
@@ -10739,7 +10715,7 @@
         <v>1246</v>
       </c>
       <c r="F188">
-        <v>2019</v>
+        <v>2022</v>
       </c>
       <c r="J188" t="s">
         <v>1247</v>
@@ -10759,7 +10735,7 @@
         <v>1250</v>
       </c>
       <c r="F189">
-        <v>2019</v>
+        <v>2022</v>
       </c>
       <c r="J189" t="s">
         <v>1251</v>
@@ -10799,7 +10775,7 @@
         <v>1258</v>
       </c>
       <c r="F191">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="J191" t="s">
         <v>1259</v>
@@ -10859,7 +10835,7 @@
         <v>1270</v>
       </c>
       <c r="F194">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="J194" t="s">
         <v>1271</v>
@@ -10879,7 +10855,7 @@
         <v>1274</v>
       </c>
       <c r="F195">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="J195" t="s">
         <v>1275</v>
@@ -10899,7 +10875,7 @@
         <v>1278</v>
       </c>
       <c r="F196">
-        <v>2023</v>
+        <v>2019</v>
       </c>
       <c r="J196" t="s">
         <v>1279</v>
@@ -10913,16 +10889,16 @@
         <v>1280</v>
       </c>
       <c r="D197" t="s">
+        <v>1265</v>
+      </c>
+      <c r="E197" t="s">
         <v>1281</v>
       </c>
-      <c r="E197" t="s">
+      <c r="F197">
+        <v>2023</v>
+      </c>
+      <c r="J197" t="s">
         <v>1282</v>
-      </c>
-      <c r="F197">
-        <v>2021</v>
-      </c>
-      <c r="J197" t="s">
-        <v>1283</v>
       </c>
       <c r="AN197" t="s">
         <v>944</v>
@@ -10930,19 +10906,19 @@
     </row>
     <row r="198" spans="3:40" x14ac:dyDescent="0.2">
       <c r="C198" t="s">
+        <v>1283</v>
+      </c>
+      <c r="D198" t="s">
         <v>1284</v>
       </c>
-      <c r="D198" t="s">
+      <c r="E198" t="s">
         <v>1285</v>
       </c>
-      <c r="E198" t="s">
+      <c r="F198">
+        <v>2021</v>
+      </c>
+      <c r="J198" t="s">
         <v>1286</v>
-      </c>
-      <c r="F198">
-        <v>2019</v>
-      </c>
-      <c r="J198" t="s">
-        <v>1287</v>
       </c>
       <c r="AN198" t="s">
         <v>944</v>
@@ -10950,19 +10926,19 @@
     </row>
     <row r="199" spans="3:40" x14ac:dyDescent="0.2">
       <c r="C199" t="s">
+        <v>1287</v>
+      </c>
+      <c r="D199" t="s">
         <v>1288</v>
       </c>
-      <c r="D199" t="s">
-        <v>1273</v>
-      </c>
       <c r="E199" t="s">
-        <v>1289</v>
+        <v>1186</v>
       </c>
       <c r="F199">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="J199" t="s">
-        <v>1290</v>
+        <v>1187</v>
       </c>
       <c r="AN199" t="s">
         <v>944</v>
@@ -10970,19 +10946,19 @@
     </row>
     <row r="200" spans="3:40" x14ac:dyDescent="0.2">
       <c r="C200" t="s">
+        <v>1289</v>
+      </c>
+      <c r="D200" t="s">
+        <v>1290</v>
+      </c>
+      <c r="E200" t="s">
         <v>1291</v>
       </c>
-      <c r="D200" t="s">
+      <c r="F200">
+        <v>2022</v>
+      </c>
+      <c r="J200" t="s">
         <v>1292</v>
-      </c>
-      <c r="E200" t="s">
-        <v>1293</v>
-      </c>
-      <c r="F200">
-        <v>2021</v>
-      </c>
-      <c r="J200" t="s">
-        <v>1294</v>
       </c>
       <c r="AN200" t="s">
         <v>944</v>
@@ -10990,39 +10966,36 @@
     </row>
     <row r="201" spans="3:40" x14ac:dyDescent="0.2">
       <c r="C201" t="s">
+        <v>1293</v>
+      </c>
+      <c r="E201" t="s">
+        <v>1294</v>
+      </c>
+      <c r="F201">
+        <v>2025</v>
+      </c>
+      <c r="J201" t="s">
         <v>1295</v>
       </c>
-      <c r="D201" t="s">
-        <v>1296</v>
-      </c>
-      <c r="E201" t="s">
-        <v>1194</v>
-      </c>
-      <c r="F201">
-        <v>2021</v>
-      </c>
-      <c r="J201" t="s">
-        <v>1195</v>
-      </c>
       <c r="AN201" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="202" spans="3:40" x14ac:dyDescent="0.2">
       <c r="C202" t="s">
+        <v>1296</v>
+      </c>
+      <c r="D202" t="s">
         <v>1297</v>
       </c>
-      <c r="D202" t="s">
+      <c r="E202" t="s">
         <v>1298</v>
       </c>
-      <c r="E202" t="s">
+      <c r="F202">
+        <v>2024</v>
+      </c>
+      <c r="J202" t="s">
         <v>1299</v>
-      </c>
-      <c r="F202">
-        <v>2022</v>
-      </c>
-      <c r="J202" t="s">
-        <v>1300</v>
       </c>
       <c r="AN202" t="s">
         <v>944</v>
@@ -11032,20 +11005,23 @@
       <c r="C203" t="s">
         <v>1301</v>
       </c>
+      <c r="D203" t="s">
+        <v>1036</v>
+      </c>
       <c r="E203" t="s">
+        <v>1300</v>
+      </c>
+      <c r="F203">
+        <v>2024</v>
+      </c>
+      <c r="J203" t="s">
         <v>1302</v>
       </c>
-      <c r="F203">
-        <v>2025</v>
-      </c>
-      <c r="J203" t="s">
-        <v>1303</v>
-      </c>
       <c r="AN203" t="s">
-        <v>943</v>
-      </c>
-    </row>
-    <row r="204" spans="3:40" x14ac:dyDescent="0.2">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="204" spans="3:40" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C204" t="s">
         <v>1304</v>
       </c>
@@ -11053,75 +11029,35 @@
         <v>1305</v>
       </c>
       <c r="E204" t="s">
+        <v>1303</v>
+      </c>
+      <c r="F204">
+        <v>2020</v>
+      </c>
+      <c r="J204" s="3" t="s">
         <v>1306</v>
       </c>
-      <c r="F204">
-        <v>2024</v>
-      </c>
-      <c r="J204" t="s">
+      <c r="AN204" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="205" spans="3:40" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C205" s="3" t="s">
+        <v>1308</v>
+      </c>
+      <c r="D205" t="s">
+        <v>816</v>
+      </c>
+      <c r="E205" t="s">
         <v>1307</v>
       </c>
-      <c r="AN204" t="s">
-        <v>944</v>
-      </c>
-    </row>
-    <row r="205" spans="3:40" x14ac:dyDescent="0.2">
-      <c r="C205" t="s">
+      <c r="F205">
+        <v>2015</v>
+      </c>
+      <c r="J205" t="s">
         <v>1309</v>
       </c>
-      <c r="D205" t="s">
-        <v>1040</v>
-      </c>
-      <c r="E205" t="s">
-        <v>1308</v>
-      </c>
-      <c r="F205">
-        <v>2024</v>
-      </c>
-      <c r="J205" t="s">
-        <v>1310</v>
-      </c>
       <c r="AN205" t="s">
-        <v>944</v>
-      </c>
-    </row>
-    <row r="206" spans="3:40" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C206" t="s">
-        <v>1312</v>
-      </c>
-      <c r="D206" t="s">
-        <v>1313</v>
-      </c>
-      <c r="E206" t="s">
-        <v>1311</v>
-      </c>
-      <c r="F206">
-        <v>2020</v>
-      </c>
-      <c r="J206" s="3" t="s">
-        <v>1314</v>
-      </c>
-      <c r="AN206" t="s">
-        <v>944</v>
-      </c>
-    </row>
-    <row r="207" spans="3:40" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C207" s="3" t="s">
-        <v>1316</v>
-      </c>
-      <c r="D207" t="s">
-        <v>816</v>
-      </c>
-      <c r="E207" t="s">
-        <v>1315</v>
-      </c>
-      <c r="F207">
-        <v>2015</v>
-      </c>
-      <c r="J207" t="s">
-        <v>1317</v>
-      </c>
-      <c r="AN207" t="s">
         <v>944</v>
       </c>
     </row>

</xml_diff>